<commit_message>
added classes for computer inventory, began work on tabs for gui
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PolycraftWorld\polycraft\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\polycraftWorkStuff\PolyCraft_Forge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
+    <workbookView minimized="1" xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -309,7 +309,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>

</xml_diff>

<commit_message>
added inventory for hospital hub
still buggy (hospital texture doesn't load and game crashes when
hospital inventory is right-clicked)
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
modified Hydroflouric acid recipe and added message upon joining game
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Desktop\polycraftWorkStuff\PolyCraft_Forge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Polycraft\PolycraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>

</xml_diff>

<commit_message>
updated excel files and tsv for 1.4.6
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -309,7 +309,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +379,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -704,7 +704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1536,7 +1536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
hot fix for sending packets to all clients instead of specific clients
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\polycraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GossStephenAndrew\workspace\UTD\Minecraft\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E695EC38-4C2F-4CEB-9BA3-BC1B51F7E48A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,15 +712,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1328125" customWidth="1"/>
+    <col min="4" max="4" width="21.59765625" customWidth="1"/>
+    <col min="5" max="5" width="22.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -736,7 +737,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -753,7 +754,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -770,7 +771,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -787,7 +788,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -804,7 +805,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -821,7 +822,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -838,7 +839,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -855,7 +856,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -872,7 +873,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -889,7 +890,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -906,7 +907,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -923,7 +924,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -940,7 +941,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -957,7 +958,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -974,7 +975,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -991,7 +992,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1008,7 +1009,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1025,7 +1026,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1042,7 +1043,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1059,7 +1060,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1076,7 +1077,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1093,7 +1094,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1110,7 +1111,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1127,7 +1128,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1144,7 +1145,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1161,7 +1162,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1178,7 +1179,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1194,7 +1195,7 @@
         <v>flashcard_m</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1210,7 +1211,7 @@
         <v>flashcard_n</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1226,7 +1227,7 @@
         <v>flashcard_o</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1242,7 +1243,7 @@
         <v>flashcard_p</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1258,7 +1259,7 @@
         <v>flashcard_q</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1274,7 +1275,7 @@
         <v>flashcard_r</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1290,7 +1291,7 @@
         <v>flashcard_s</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1306,7 +1307,7 @@
         <v>flashcard_t</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1322,7 +1323,7 @@
         <v>flashcard_u</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1338,7 +1339,7 @@
         <v>flashcard_v</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1354,7 +1355,7 @@
         <v>flashcard_w</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1370,7 +1371,7 @@
         <v>flashcard_x</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1386,7 +1387,7 @@
         <v>flashcard_y</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1402,7 +1403,7 @@
         <v>flashcard_z</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1418,7 +1419,7 @@
         <v>flashcard_p_orbital</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1434,7 +1435,7 @@
         <v>flashcard_sp</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1450,7 +1451,7 @@
         <v>flashcard_sp2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1466,7 +1467,7 @@
         <v>flashcard_sp3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1482,7 +1483,7 @@
         <v>flashcard_sp3d</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1498,7 +1499,7 @@
         <v>flashcard_sp3d2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1514,7 +1515,7 @@
         <v>flashcard_trans</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1543,15 +1544,15 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1328125" customWidth="1"/>
+    <col min="4" max="4" width="21.59765625" customWidth="1"/>
+    <col min="5" max="5" width="22.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -1568,7 +1569,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1585,262 +1586,262 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="D49" s="6"/>

</xml_diff>

<commit_message>
Steam cracker recipe fixes
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GossStephenAndrew\workspace\UTD\Minecraft\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\polycraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E695EC38-4C2F-4CEB-9BA3-BC1B51F7E48A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D9FA66-2DD1-411B-9D22-907C792FA13F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -712,15 +712,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1328125" customWidth="1"/>
-    <col min="4" max="4" width="21.59765625" customWidth="1"/>
-    <col min="5" max="5" width="22.73046875" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -737,7 +737,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -754,7 +754,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -771,7 +771,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -788,7 +788,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -805,7 +805,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -822,7 +822,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -839,7 +839,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -856,7 +856,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -873,7 +873,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -890,7 +890,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -907,7 +907,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -924,7 +924,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -941,7 +941,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -958,7 +958,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -975,7 +975,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -992,7 +992,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1195,7 +1195,7 @@
         <v>flashcard_m</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1211,7 +1211,7 @@
         <v>flashcard_n</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1227,7 +1227,7 @@
         <v>flashcard_o</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1243,7 +1243,7 @@
         <v>flashcard_p</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1259,7 +1259,7 @@
         <v>flashcard_q</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1275,7 +1275,7 @@
         <v>flashcard_r</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1291,7 +1291,7 @@
         <v>flashcard_s</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1307,7 +1307,7 @@
         <v>flashcard_t</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1323,7 +1323,7 @@
         <v>flashcard_u</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1339,7 +1339,7 @@
         <v>flashcard_v</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1355,7 +1355,7 @@
         <v>flashcard_w</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1371,7 +1371,7 @@
         <v>flashcard_x</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1387,7 +1387,7 @@
         <v>flashcard_y</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1403,7 +1403,7 @@
         <v>flashcard_z</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1419,7 +1419,7 @@
         <v>flashcard_p_orbital</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1435,7 +1435,7 @@
         <v>flashcard_sp</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1451,7 +1451,7 @@
         <v>flashcard_sp2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1467,7 +1467,7 @@
         <v>flashcard_sp3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1483,7 +1483,7 @@
         <v>flashcard_sp3d</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1499,7 +1499,7 @@
         <v>flashcard_sp3d2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1515,7 +1515,7 @@
         <v>flashcard_trans</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1544,15 +1544,15 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1328125" customWidth="1"/>
-    <col min="4" max="4" width="21.59765625" customWidth="1"/>
-    <col min="5" max="5" width="22.73046875" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1586,262 +1586,262 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="D49" s="6"/>

</xml_diff>

<commit_message>
Added synthetic grips to polycraft tools.
Buffed up polycraft tools to be better than diamond tools.
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\polycraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Seeligson\Desktop\PolycraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D9FA66-2DD1-411B-9D22-907C792FA13F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -310,7 +309,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,7 +379,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -705,7 +704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1537,7 +1536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
Added new test dimension and password door
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Seeligson\Desktop\PolycraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Polycraft\PolycraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA911D40-2ECE-4E94-AA76-38F1BD4EBAD0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
+    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -309,7 +310,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +380,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -704,7 +705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1536,7 +1537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
change a few recipies
refueling jet packs can now be done in a 2x2 grid
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Seeligson\Desktop\PolycraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GossStephenAndrew\workspace\UTD\Minecraft\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4BD5B1-350F-47D5-B2AF-72108E3FD81E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
+    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -309,7 +310,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +380,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -704,22 +705,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1328125" customWidth="1"/>
+    <col min="4" max="4" width="21.59765625" customWidth="1"/>
+    <col min="5" max="5" width="22.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -736,7 +737,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -753,7 +754,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -770,7 +771,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -787,7 +788,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -804,7 +805,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -821,7 +822,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -838,7 +839,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -855,7 +856,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -872,7 +873,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -889,7 +890,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -906,7 +907,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -923,7 +924,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -940,7 +941,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -957,7 +958,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -974,7 +975,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -991,7 +992,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1008,7 +1009,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1025,7 +1026,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1042,7 +1043,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1059,7 +1060,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1076,7 +1077,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1093,7 +1094,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1110,7 +1111,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1127,7 +1128,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1144,7 +1145,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1161,7 +1162,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1178,7 +1179,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1194,7 +1195,7 @@
         <v>flashcard_m</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1210,7 +1211,7 @@
         <v>flashcard_n</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1226,7 +1227,7 @@
         <v>flashcard_o</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1242,7 +1243,7 @@
         <v>flashcard_p</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1258,7 +1259,7 @@
         <v>flashcard_q</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1274,7 +1275,7 @@
         <v>flashcard_r</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1290,7 +1291,7 @@
         <v>flashcard_s</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1306,7 +1307,7 @@
         <v>flashcard_t</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1322,7 +1323,7 @@
         <v>flashcard_u</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1338,7 +1339,7 @@
         <v>flashcard_v</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1354,7 +1355,7 @@
         <v>flashcard_w</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1370,7 +1371,7 @@
         <v>flashcard_x</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1386,7 +1387,7 @@
         <v>flashcard_y</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1402,7 +1403,7 @@
         <v>flashcard_z</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1418,7 +1419,7 @@
         <v>flashcard_p_orbital</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1434,7 +1435,7 @@
         <v>flashcard_sp</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1450,7 +1451,7 @@
         <v>flashcard_sp2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1466,7 +1467,7 @@
         <v>flashcard_sp3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1482,7 +1483,7 @@
         <v>flashcard_sp3d</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1498,7 +1499,7 @@
         <v>flashcard_sp3d2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1514,7 +1515,7 @@
         <v>flashcard_trans</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1536,22 +1537,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1328125" customWidth="1"/>
+    <col min="4" max="4" width="21.59765625" customWidth="1"/>
+    <col min="5" max="5" width="22.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -1568,7 +1569,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1585,262 +1586,262 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="D49" s="6"/>

</xml_diff>

<commit_message>
Added Entities OilSlime(dropped items don't stack), Dummy
Added PolyMaterialOil Not implemented

Fixed PolyCraft EntityEggs
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GossStephenAndrew\workspace\UTD\Minecraft\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4BD5B1-350F-47D5-B2AF-72108E3FD81E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91F5BC1-3FD7-4C56-943E-8234D6BE22F3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -412,6 +412,11 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>State of Matter</v>
+          </cell>
+        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -430,14 +435,62 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Item</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Block</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Element</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Mineral</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Alloy</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Version</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Version</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="9">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Polymer Object</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -712,15 +765,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1328125" customWidth="1"/>
-    <col min="4" max="4" width="21.59765625" customWidth="1"/>
-    <col min="5" max="5" width="22.73046875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -737,7 +790,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -754,7 +807,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -771,7 +824,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -788,7 +841,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -805,7 +858,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -822,7 +875,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -839,7 +892,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -856,7 +909,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -873,7 +926,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -890,7 +943,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -907,7 +960,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -924,7 +977,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -941,7 +994,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -958,7 +1011,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -975,7 +1028,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -992,7 +1045,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1009,7 +1062,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1026,7 +1079,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1043,7 +1096,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1060,7 +1113,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1077,7 +1130,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1094,7 +1147,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1111,7 +1164,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1128,7 +1181,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1145,7 +1198,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1162,7 +1215,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1179,7 +1232,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1195,7 +1248,7 @@
         <v>flashcard_m</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1211,7 +1264,7 @@
         <v>flashcard_n</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1227,7 +1280,7 @@
         <v>flashcard_o</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1243,7 +1296,7 @@
         <v>flashcard_p</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1259,7 +1312,7 @@
         <v>flashcard_q</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1275,7 +1328,7 @@
         <v>flashcard_r</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1291,7 +1344,7 @@
         <v>flashcard_s</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1307,7 +1360,7 @@
         <v>flashcard_t</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1323,7 +1376,7 @@
         <v>flashcard_u</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1339,7 +1392,7 @@
         <v>flashcard_v</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1355,7 +1408,7 @@
         <v>flashcard_w</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1371,7 +1424,7 @@
         <v>flashcard_x</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1387,7 +1440,7 @@
         <v>flashcard_y</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1403,7 +1456,7 @@
         <v>flashcard_z</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1419,7 +1472,7 @@
         <v>flashcard_p_orbital</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1435,7 +1488,7 @@
         <v>flashcard_sp</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1451,7 +1504,7 @@
         <v>flashcard_sp2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1467,7 +1520,7 @@
         <v>flashcard_sp3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1483,7 +1536,7 @@
         <v>flashcard_sp3d</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1499,7 +1552,7 @@
         <v>flashcard_sp3d2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1515,7 +1568,7 @@
         <v>flashcard_trans</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1544,15 +1597,15 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1328125" customWidth="1"/>
-    <col min="4" max="4" width="21.59765625" customWidth="1"/>
-    <col min="5" max="5" width="22.73046875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -1569,7 +1622,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1586,262 +1639,262 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="D49" s="6"/>

</xml_diff>

<commit_message>
Created Constitution Claim Custom item
Created Super Ink Custom item

Fixed Schematics
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91F5BC1-3FD7-4C56-943E-8234D6BE22F3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CCAB36-0108-4A7D-9ED5-0238D7E62977}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -412,11 +412,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>State of Matter</v>
-          </cell>
-        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -435,62 +430,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Minecraft Item</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Minecraft Block</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Element</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Mineral</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Alloy</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Version</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Version</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Polymer Object</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>

<commit_message>
Dev tool can now 'paste' and 'fill'
New PolyPortal Block

fixed issue with Temp PrivateProperties not setting Permissions
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CCAB36-0108-4A7D-9ED5-0238D7E62977}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29966155-602E-4958-8001-6BCAB5217AE9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Can send data to portal with Constitution Claim
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CCAB36-0108-4A7D-9ED5-0238D7E62977}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BD55B7-ABF5-4BCB-B911-A83902DD090F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
Added KillWall Command and Game Command
Added Game Block
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91F5BC1-3FD7-4C56-943E-8234D6BE22F3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19C4B4D-244A-4D96-959E-F9A73F39C620}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -412,11 +412,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>State of Matter</v>
-          </cell>
-        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -435,62 +430,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Minecraft Item</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Minecraft Block</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Element</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Mineral</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Alloy</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Version</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Version</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Polymer Object</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>

<commit_message>
Reserved item IDs for TextWall, KBB, FKBB, and cleats
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Polycraft\Documents\Polycraft Forge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AEC4FA-C2D4-470B-9D13-4002C169EF19}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A6FA5453-E496-46D6-814B-2566E21DDF14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -412,11 +412,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>State of Matter</v>
-          </cell>
-        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -435,62 +430,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Minecraft Item</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Minecraft Block</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Element</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Mineral</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Alloy</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Version</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Version</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Polymer Object</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -765,15 +712,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -790,7 +737,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -807,7 +754,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -824,7 +771,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -841,7 +788,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -858,7 +805,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -875,7 +822,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -892,7 +839,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -909,7 +856,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -926,7 +873,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -943,7 +890,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -960,7 +907,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -977,7 +924,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -994,7 +941,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1011,7 +958,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1028,7 +975,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1045,7 +992,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1062,7 +1009,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1079,7 +1026,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1096,7 +1043,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1113,7 +1060,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1130,7 +1077,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1147,7 +1094,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1164,7 +1111,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1181,7 +1128,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1198,7 +1145,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1215,7 +1162,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1232,7 +1179,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1248,7 +1195,7 @@
         <v>flashcard_m</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1264,7 +1211,7 @@
         <v>flashcard_n</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1280,7 +1227,7 @@
         <v>flashcard_o</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1296,7 +1243,7 @@
         <v>flashcard_p</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1312,7 +1259,7 @@
         <v>flashcard_q</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1328,7 +1275,7 @@
         <v>flashcard_r</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1344,7 +1291,7 @@
         <v>flashcard_s</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1360,7 +1307,7 @@
         <v>flashcard_t</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1376,7 +1323,7 @@
         <v>flashcard_u</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1392,7 +1339,7 @@
         <v>flashcard_v</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1408,7 +1355,7 @@
         <v>flashcard_w</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1424,7 +1371,7 @@
         <v>flashcard_x</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1440,7 +1387,7 @@
         <v>flashcard_y</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1456,7 +1403,7 @@
         <v>flashcard_z</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1472,7 +1419,7 @@
         <v>flashcard_p_orbital</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1488,7 +1435,7 @@
         <v>flashcard_sp</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1504,7 +1451,7 @@
         <v>flashcard_sp2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1520,7 +1467,7 @@
         <v>flashcard_sp3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1536,7 +1483,7 @@
         <v>flashcard_sp3d</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1552,7 +1499,7 @@
         <v>flashcard_sp3d2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1568,7 +1515,7 @@
         <v>flashcard_trans</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1597,15 +1544,15 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -1622,7 +1569,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1639,262 +1586,262 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="D49" s="6"/>

</xml_diff>

<commit_message>
Created Consent Entity Hanging Objects
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Polycraft\Documents\Polycraft Forge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Triforce\Documents\polycraftworld\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{74612F9F-2C22-4B6D-9DB8-831199B81861}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B4A48A9C-E56B-4C30-944F-F2777ECAFFC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
added polycrafting table and CTB recipies
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Triforce\Documents\polycraftworld\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxg115630\polycraft forge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F2AA2852-7CF8-458C-9521-CA3CEE3F8803}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -310,7 +309,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,7 +379,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -705,7 +704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1537,7 +1536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
Added Cannons and EntityIronCannonBall
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxg115630\polycraft forge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{29BFC989-1448-4BE1-BAD4-57279FCEEE59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" firstSheet="1" activeTab="1"/>
+    <workbookView minimized="1" xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -18,10 +19,17 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -309,7 +317,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +387,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -411,6 +419,11 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>State of Matter</v>
+          </cell>
+        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -429,14 +442,62 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Item</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Block</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Element</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Mineral</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Alloy</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Version</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Version</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="9">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Polymer Object</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -704,22 +765,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -736,7 +797,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -753,7 +814,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -770,7 +831,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -787,7 +848,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -804,7 +865,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -821,7 +882,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -838,7 +899,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -855,7 +916,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -872,7 +933,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -889,7 +950,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -906,7 +967,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -923,7 +984,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -940,7 +1001,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -957,7 +1018,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -974,7 +1035,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -991,7 +1052,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1008,7 +1069,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1025,7 +1086,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1042,7 +1103,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1059,7 +1120,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1076,7 +1137,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1093,7 +1154,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1110,7 +1171,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1127,7 +1188,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1144,7 +1205,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1161,7 +1222,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1178,7 +1239,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1194,7 +1255,7 @@
         <v>flashcard_m</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1210,7 +1271,7 @@
         <v>flashcard_n</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1226,7 +1287,7 @@
         <v>flashcard_o</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1242,7 +1303,7 @@
         <v>flashcard_p</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1258,7 +1319,7 @@
         <v>flashcard_q</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1274,7 +1335,7 @@
         <v>flashcard_r</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1290,7 +1351,7 @@
         <v>flashcard_s</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1306,7 +1367,7 @@
         <v>flashcard_t</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1322,7 +1383,7 @@
         <v>flashcard_u</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1338,7 +1399,7 @@
         <v>flashcard_v</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1354,7 +1415,7 @@
         <v>flashcard_w</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1370,7 +1431,7 @@
         <v>flashcard_x</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1386,7 +1447,7 @@
         <v>flashcard_y</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1402,7 +1463,7 @@
         <v>flashcard_z</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1418,7 +1479,7 @@
         <v>flashcard_p_orbital</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1434,7 +1495,7 @@
         <v>flashcard_sp</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1450,7 +1511,7 @@
         <v>flashcard_sp2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1466,7 +1527,7 @@
         <v>flashcard_sp3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1482,7 +1543,7 @@
         <v>flashcard_sp3d</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1498,7 +1559,7 @@
         <v>flashcard_sp3d2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1514,7 +1575,7 @@
         <v>flashcard_trans</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1536,22 +1597,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>[1]Enums!$A$133</f>
         <v>Version</v>
@@ -1568,7 +1629,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="str">
         <f>[1]Enums!$A$162</f>
         <v>1.4.3</v>
@@ -1585,262 +1646,262 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="D49" s="6"/>

</xml_diff>

<commit_message>
Created mining hammer that breaks a 3x3x3 block around focused block.
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxg115630\polycraft forge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRZ170000\Desktop\polycraftforge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" firstSheet="1" activeTab="1"/>
+    <workbookView minimized="1" xWindow="2235" yWindow="0" windowWidth="20400" windowHeight="8745" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -411,6 +411,11 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>State of Matter</v>
+          </cell>
+        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -429,14 +434,62 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Item</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Block</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Element</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Mineral</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Alloy</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Version</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Version</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="9">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Polymer Object</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1540,7 +1593,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="R20" sqref="R19:R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cannons now have an __**incomplete**__ GUI
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29BFC989-1448-4BE1-BAD4-57279FCEEE59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113926B7-610E-40DE-8422-A158723F0D6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="0" windowWidth="20400" windowHeight="8748" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flashcard" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -419,11 +418,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>State of Matter</v>
-          </cell>
-        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -442,62 +436,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Minecraft Item</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Minecraft Block</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Element</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Mineral</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Alloy</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Version</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Version</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Polymer Object</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>

<commit_message>
Slingshot exists and shoots invisible paintball arrows.
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjg150230\PolycraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRZ170000\Desktop\polycraftforge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1540,7 +1540,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
/color changes color, paint now colors wool, the cube knows all
</commit_message>
<xml_diff>
--- a/config/Polycraft Learning.xlsx
+++ b/config/Polycraft Learning.xlsx
@@ -411,6 +411,11 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>State of Matter</v>
+          </cell>
+        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -429,14 +434,62 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Item</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Block</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Element</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Mineral</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Alloy</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Version</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Version</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="9">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Polymer Object</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>